<commit_message>
Na aanlign van vergadering met NEL
</commit_message>
<xml_diff>
--- a/Excels/TempData.xlsx
+++ b/Excels/TempData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="8652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="8652"/>
   </bookViews>
   <sheets>
     <sheet name="All Sets" sheetId="2" r:id="rId1"/>
@@ -418,21 +418,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -467,6 +452,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,7 +783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L492"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B45" sqref="B45:B60"/>
     </sheetView>
@@ -13602,7 +13602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -13624,123 +13624,123 @@
     <col min="21" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:20" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="H2" s="18" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="H2" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="18" t="s">
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="H3" s="21" t="s">
+      <c r="F3" s="38"/>
+      <c r="H3" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="21" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="N3" s="21" t="s">
+      <c r="L3" s="38"/>
+      <c r="N3" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="22"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="21" t="s">
+      <c r="O3" s="38"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="22"/>
+      <c r="R3" s="38"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="22" t="s">
         <v>44</v>
       </c>
       <c r="J4" s="16"/>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="N4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="R4" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="29">
+      <c r="B5" s="24">
         <v>37.272114000000002</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="25">
         <v>36.700000000000003</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="36">
+      <c r="E5" s="31">
         <v>36.953676999999999</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="29">
         <v>36.4</v>
       </c>
       <c r="H5" s="11">
         <v>32.81</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="19">
         <v>37.6</v>
       </c>
       <c r="J5" s="16"/>
-      <c r="K5" s="24">
+      <c r="K5" s="19">
         <v>33.840000000000003</v>
       </c>
       <c r="L5" s="12">
@@ -13749,10 +13749,10 @@
       <c r="N5" s="11">
         <v>33.56</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="18">
         <v>37.6</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="18">
         <v>34.44</v>
       </c>
       <c r="R5" s="12">
@@ -13760,27 +13760,27 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="29">
+      <c r="B6" s="24">
         <v>37.247281999999998</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="25">
         <v>37.700000000000003</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="11">
         <v>36.769891000000001</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="25">
         <v>37.4</v>
       </c>
       <c r="H6" s="11">
         <v>32.840000000000003</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="19">
         <v>38.4</v>
       </c>
       <c r="J6" s="16"/>
-      <c r="K6" s="24">
+      <c r="K6" s="19">
         <v>33.840000000000003</v>
       </c>
       <c r="L6" s="12">
@@ -13789,10 +13789,10 @@
       <c r="N6" s="11">
         <v>33.590000000000003</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="19">
         <v>38.299999999999997</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="19">
         <v>34.44</v>
       </c>
       <c r="R6" s="12">
@@ -13800,27 +13800,27 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B7" s="29">
+      <c r="B7" s="24">
         <v>37.326957</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="25">
         <v>37.6</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="11">
         <v>36.806792999999999</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="25">
         <v>37.4</v>
       </c>
       <c r="H7" s="11">
         <v>32.909999999999997</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="19">
         <v>38.200000000000003</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="24">
+      <c r="K7" s="19">
         <v>33.880000000000003</v>
       </c>
       <c r="L7" s="12">
@@ -13829,10 +13829,10 @@
       <c r="N7" s="11">
         <v>33.630000000000003</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="19">
         <v>38.4</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="Q7" s="19">
         <v>34.44</v>
       </c>
       <c r="R7" s="12">
@@ -13840,338 +13840,338 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="29">
+      <c r="B8" s="24">
         <v>37.363278999999999</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="15"/>
       <c r="E8" s="11">
         <v>36.837434000000002</v>
       </c>
-      <c r="F8" s="30"/>
+      <c r="F8" s="25"/>
       <c r="H8" s="11">
         <v>32.94</v>
       </c>
-      <c r="I8" s="24"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="16"/>
-      <c r="K8" s="24">
+      <c r="K8" s="19">
         <v>33.880000000000003</v>
       </c>
       <c r="L8" s="12"/>
       <c r="N8" s="11">
         <v>33.659999999999997</v>
       </c>
-      <c r="O8" s="24"/>
-      <c r="Q8" s="24">
+      <c r="O8" s="19"/>
+      <c r="Q8" s="19">
         <v>34.47</v>
       </c>
       <c r="R8" s="12"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B9" s="29">
+      <c r="B9" s="24">
         <v>37.390123000000003</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="15"/>
       <c r="E9" s="11">
         <v>37.411717000000003</v>
       </c>
-      <c r="F9" s="30"/>
+      <c r="F9" s="25"/>
       <c r="H9" s="11">
         <v>32.97</v>
       </c>
-      <c r="I9" s="24"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="16"/>
-      <c r="K9" s="24">
+      <c r="K9" s="19">
         <v>33.909999999999997</v>
       </c>
       <c r="L9" s="12"/>
       <c r="N9" s="11">
         <v>33.69</v>
       </c>
-      <c r="O9" s="24"/>
-      <c r="Q9" s="24">
+      <c r="O9" s="19"/>
+      <c r="Q9" s="19">
         <v>34.47</v>
       </c>
       <c r="R9" s="12"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="29">
+      <c r="B10" s="24">
         <v>37.350126000000003</v>
       </c>
-      <c r="C10" s="30"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="15"/>
       <c r="E10" s="11">
         <v>38.336865000000003</v>
       </c>
-      <c r="F10" s="30"/>
+      <c r="F10" s="25"/>
       <c r="H10" s="11">
         <v>33</v>
       </c>
-      <c r="I10" s="24"/>
+      <c r="I10" s="19"/>
       <c r="J10" s="16"/>
-      <c r="K10" s="24">
+      <c r="K10" s="19">
         <v>33.909999999999997</v>
       </c>
       <c r="L10" s="12"/>
       <c r="N10" s="11">
         <v>33.72</v>
       </c>
-      <c r="O10" s="24"/>
-      <c r="Q10" s="24">
+      <c r="O10" s="19"/>
+      <c r="Q10" s="19">
         <v>34.47</v>
       </c>
       <c r="R10" s="12"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="29">
+      <c r="B11" s="24">
         <v>37.340676000000002</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="15"/>
       <c r="E11" s="11">
         <v>38.149436999999999</v>
       </c>
-      <c r="F11" s="30"/>
+      <c r="F11" s="25"/>
       <c r="H11" s="11">
         <v>33.03</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="19"/>
       <c r="J11" s="16"/>
-      <c r="K11" s="24">
+      <c r="K11" s="19">
         <v>33.94</v>
       </c>
       <c r="L11" s="12"/>
       <c r="N11" s="11">
         <v>33.75</v>
       </c>
-      <c r="O11" s="24"/>
-      <c r="Q11" s="24">
+      <c r="O11" s="19"/>
+      <c r="Q11" s="19">
         <v>34.5</v>
       </c>
       <c r="R11" s="12"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="29">
+      <c r="B12" s="24">
         <v>37.588124000000001</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="15"/>
       <c r="E12" s="11">
         <v>38.052551999999999</v>
       </c>
-      <c r="F12" s="30"/>
+      <c r="F12" s="25"/>
       <c r="H12" s="11">
         <v>33.06</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="19"/>
       <c r="J12" s="16"/>
-      <c r="K12" s="24">
+      <c r="K12" s="19">
         <v>33.94</v>
       </c>
       <c r="L12" s="12"/>
       <c r="N12" s="11">
         <v>33.78</v>
       </c>
-      <c r="O12" s="24"/>
-      <c r="Q12" s="24">
+      <c r="O12" s="19"/>
+      <c r="Q12" s="19">
         <v>34.5</v>
       </c>
       <c r="R12" s="12"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="29">
+      <c r="B13" s="24">
         <v>37.493138000000002</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="15"/>
       <c r="E13" s="11">
         <v>37.931345</v>
       </c>
-      <c r="F13" s="30"/>
+      <c r="F13" s="25"/>
       <c r="H13" s="11">
         <v>33.090000000000003</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="19"/>
       <c r="J13" s="16"/>
-      <c r="K13" s="24">
+      <c r="K13" s="19">
         <v>33.94</v>
       </c>
       <c r="L13" s="12"/>
       <c r="N13" s="11">
         <v>33.81</v>
       </c>
-      <c r="O13" s="24"/>
-      <c r="Q13" s="24">
+      <c r="O13" s="19"/>
+      <c r="Q13" s="19">
         <v>34.53</v>
       </c>
       <c r="R13" s="12"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="29">
+      <c r="B14" s="24">
         <v>37.493138000000002</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="15"/>
       <c r="E14" s="11">
         <v>37.359831999999997</v>
       </c>
-      <c r="F14" s="30"/>
+      <c r="F14" s="25"/>
       <c r="H14" s="11">
         <v>33.130000000000003</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="19"/>
       <c r="J14" s="16"/>
-      <c r="K14" s="24">
+      <c r="K14" s="19">
         <v>33.97</v>
       </c>
       <c r="L14" s="12"/>
       <c r="N14" s="11">
         <v>33.840000000000003</v>
       </c>
-      <c r="O14" s="24"/>
-      <c r="Q14" s="24">
+      <c r="O14" s="19"/>
+      <c r="Q14" s="19">
         <v>34.53</v>
       </c>
       <c r="R14" s="12"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B15" s="29">
+      <c r="B15" s="24">
         <v>37.544719999999998</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="15"/>
       <c r="E15" s="11">
         <v>37.442180999999998</v>
       </c>
-      <c r="F15" s="30"/>
+      <c r="F15" s="25"/>
       <c r="H15" s="11">
         <v>33.159999999999997</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="19"/>
       <c r="J15" s="16"/>
-      <c r="K15" s="24">
+      <c r="K15" s="19">
         <v>33.97</v>
       </c>
       <c r="L15" s="12"/>
       <c r="N15" s="11">
         <v>33.880000000000003</v>
       </c>
-      <c r="O15" s="24"/>
-      <c r="Q15" s="24">
+      <c r="O15" s="19"/>
+      <c r="Q15" s="19">
         <v>34.53</v>
       </c>
       <c r="R15" s="12"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="29">
+      <c r="B16" s="24">
         <v>37.733241999999997</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="15"/>
       <c r="E16" s="11">
         <v>37.448355999999997</v>
       </c>
-      <c r="F16" s="30"/>
+      <c r="F16" s="25"/>
       <c r="H16" s="11">
         <v>33.19</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="19"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="24">
+      <c r="K16" s="19">
         <v>33.97</v>
       </c>
       <c r="L16" s="12"/>
       <c r="N16" s="11">
         <v>33.909999999999997</v>
       </c>
-      <c r="O16" s="24"/>
-      <c r="Q16" s="24">
+      <c r="O16" s="19"/>
+      <c r="Q16" s="19">
         <v>34.53</v>
       </c>
       <c r="R16" s="12"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="29">
+      <c r="B17" s="24">
         <v>37.565821999999997</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="15"/>
       <c r="E17" s="11">
         <v>37.767651999999998</v>
       </c>
-      <c r="F17" s="30"/>
+      <c r="F17" s="25"/>
       <c r="H17" s="11">
         <v>33.22</v>
       </c>
-      <c r="I17" s="24"/>
+      <c r="I17" s="19"/>
       <c r="J17" s="16"/>
-      <c r="K17" s="24">
+      <c r="K17" s="19">
         <v>33.97</v>
       </c>
       <c r="L17" s="12"/>
       <c r="N17" s="11">
         <v>33.909999999999997</v>
       </c>
-      <c r="O17" s="24"/>
-      <c r="Q17" s="24">
+      <c r="O17" s="19"/>
+      <c r="Q17" s="19">
         <v>34.56</v>
       </c>
       <c r="R17" s="12"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="29">
+      <c r="B18" s="24">
         <v>37.541235</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="15"/>
       <c r="E18" s="11">
         <v>37.500210000000003</v>
       </c>
-      <c r="F18" s="30"/>
+      <c r="F18" s="25"/>
       <c r="H18" s="11">
         <v>33.25</v>
       </c>
-      <c r="I18" s="24"/>
+      <c r="I18" s="19"/>
       <c r="J18" s="16"/>
-      <c r="K18" s="24">
+      <c r="K18" s="19">
         <v>34</v>
       </c>
       <c r="L18" s="12"/>
       <c r="N18" s="11">
         <v>33.94</v>
       </c>
-      <c r="O18" s="24"/>
-      <c r="Q18" s="24">
+      <c r="O18" s="19"/>
+      <c r="Q18" s="19">
         <v>34.56</v>
       </c>
       <c r="R18" s="12"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="31">
+      <c r="B19" s="26">
         <v>37.495519000000002</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="13">
         <v>37.500210000000003</v>
       </c>
-      <c r="F19" s="32"/>
+      <c r="F19" s="27"/>
       <c r="H19" s="13">
         <v>33.28</v>
       </c>
-      <c r="I19" s="25"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="25">
+      <c r="K19" s="20">
         <v>34</v>
       </c>
       <c r="L19" s="14"/>
       <c r="N19" s="13">
         <v>33.97</v>
       </c>
-      <c r="O19" s="25"/>
+      <c r="O19" s="20"/>
       <c r="P19" s="17"/>
-      <c r="Q19" s="25">
+      <c r="Q19" s="20">
         <v>34.56</v>
       </c>
       <c r="R19" s="14"/>

</xml_diff>